<commit_message>
EDA dendrogram added, pipeline update, algorithm evaluation ipynb updated
Added:
 - EDA dendrogram of feature clusters
 - img subfolder for visualizations

Updated:
 - rank_eval ipynb - testing out results of ReliefF, mutual info, testing jaccard vs fuji
 - rank_eval pipeline (added eval func with logging, rank timing, fuzzy_jaccard now default eval algo)
 - added new results to documentation
</commit_message>
<xml_diff>
--- a/src/documentation/Feature Ranking Documentation.xlsx
+++ b/src/documentation/Feature Ranking Documentation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>FEATURE</t>
   </si>
@@ -43,13 +43,19 @@
     <t>Algorithm tested</t>
   </si>
   <si>
-    <t>Score (singles, first_gen)</t>
+    <t>Evaluation method</t>
+  </si>
+  <si>
+    <t>Evaluation Score (singles, first_gen)</t>
   </si>
   <si>
     <t>notes &amp; observations</t>
   </si>
   <si>
     <t>Mutual information, all data</t>
+  </si>
+  <si>
+    <t>fuji</t>
   </si>
   <si>
     <t>(0.8635530367032218, 0.7392145047450169)</t>
@@ -59,6 +65,9 @@
   </si>
   <si>
     <t>(0.7004396806244233, 0.6393842363753732)</t>
+  </si>
+  <si>
+    <t>only top 10 taken from scores</t>
   </si>
   <si>
     <t>ReliefF, 0.1% of data randomly sampled</t>
@@ -78,6 +87,63 @@
   <si>
     <t>(0.8514649310560692, 0.7461393376478086)</t>
   </si>
+  <si>
+    <t>ReliefF, 33% of data randomly sampled</t>
+  </si>
+  <si>
+    <t>(0.8451238848308656, 0.7523493111288934)</t>
+  </si>
+  <si>
+    <t>jaccard</t>
+  </si>
+  <si>
+    <t>(0.4194700441858172, 0.43152862233540834)</t>
+  </si>
+  <si>
+    <t>(0.40036216514472456, 0.4187043577708233)</t>
+  </si>
+  <si>
+    <t>(0.4218725932651735, 0.4180492488316388)</t>
+  </si>
+  <si>
+    <t>(0.39261719106970383, 0.415318234240222)</t>
+  </si>
+  <si>
+    <t>Mutual info, 100 x sampled(n=15,000)</t>
+  </si>
+  <si>
+    <t>0.428 ± 0.015, 0.588 ± 0.018</t>
+  </si>
+  <si>
+    <t>cca 4s for a single ranking</t>
+  </si>
+  <si>
+    <t>Mutual info, 10 x sampled(n=150,000)</t>
+  </si>
+  <si>
+    <t>0.434 ± 0.010, 0.585 ± 0.011</t>
+  </si>
+  <si>
+    <t>cca 50s for a single rank</t>
+  </si>
+  <si>
+    <t>Mutual info, all</t>
+  </si>
+  <si>
+    <t>0.437, 0.522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">785s </t>
+  </si>
+  <si>
+    <t>0.805 ± 0.011, 0.837 ± 0.014</t>
+  </si>
+  <si>
+    <t>0.809 ± 0.011, 0.826 ± 0.007</t>
+  </si>
+  <si>
+    <t>0.794, 0.783</t>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +152,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -128,6 +194,22 @@
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FFA5A5A5"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -189,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -213,13 +295,13 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
@@ -231,6 +313,9 @@
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -240,10 +325,25 @@
     <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -522,10 +622,10 @@
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>98.0</v>
+        <v>0.0</v>
       </c>
       <c r="B2" s="6">
-        <v>2.0</v>
+        <v>295.0</v>
       </c>
       <c r="C2" s="7">
         <f t="shared" ref="C2:C102" si="1">IF(B2&gt;1000, 1, 0)</f>
@@ -534,46 +634,42 @@
       <c r="D2" s="6">
         <v>0.0</v>
       </c>
-      <c r="E2" s="8">
-        <v>4.0</v>
-      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="9">
-        <v>0.94</v>
+        <v>0.740219693124285</v>
       </c>
       <c r="G2" s="9">
-        <v>0.998550282879953</v>
+        <v>0.0769716906460384</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>99.0</v>
+        <v>1.0</v>
       </c>
       <c r="B3" s="6">
-        <v>2.0</v>
+        <v>2526.0</v>
       </c>
       <c r="C3" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="6">
         <v>0.0</v>
       </c>
-      <c r="E3" s="8">
-        <v>4.0</v>
-      </c>
+      <c r="E3" s="8"/>
       <c r="F3" s="9">
-        <v>0.94</v>
+        <v>0.748215743402743</v>
       </c>
       <c r="G3" s="9">
-        <v>0.998550282879953</v>
+        <v>0.147141781022099</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B4" s="6">
-        <v>14633.0</v>
+        <v>39404.0</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" si="1"/>
@@ -589,39 +685,39 @@
         <v>0.763096570342066</v>
       </c>
       <c r="G4" s="9">
-        <v>0.238650147201154</v>
+        <v>0.0297189739520529</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>29.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" s="6">
-        <v>51.0</v>
+        <v>14633.0</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" s="6">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
       <c r="F5" s="9">
-        <v>0.744694738885608</v>
+        <v>0.763096570342066</v>
       </c>
       <c r="G5" s="9">
-        <v>0.187370761019425</v>
+        <v>0.238650147201154</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>87.0</v>
+        <v>4.0</v>
       </c>
       <c r="B6" s="6">
-        <v>749.0</v>
+        <v>2.0</v>
       </c>
       <c r="C6" s="7">
         <f t="shared" si="1"/>
@@ -630,22 +726,20 @@
       <c r="D6" s="6">
         <v>0.0</v>
       </c>
-      <c r="E6" s="6">
-        <v>2.0</v>
-      </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="9">
-        <v>0.741184783827072</v>
+        <v>0.739754248150703</v>
       </c>
       <c r="G6" s="9">
-        <v>0.186470416672814</v>
+        <v>0.0266328097093283</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>86.0</v>
+        <v>5.0</v>
       </c>
       <c r="B7" s="6">
-        <v>743.0</v>
+        <v>2.0</v>
       </c>
       <c r="C7" s="7">
         <f t="shared" si="1"/>
@@ -654,46 +748,42 @@
       <c r="D7" s="6">
         <v>0.0</v>
       </c>
-      <c r="E7" s="6">
-        <v>2.0</v>
-      </c>
+      <c r="E7" s="8"/>
       <c r="F7" s="9">
-        <v>0.741128845343718</v>
+        <v>0.74211166919656</v>
       </c>
       <c r="G7" s="9">
-        <v>0.186466811988465</v>
+        <v>0.0216277064894057</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
       <c r="B8" s="6">
-        <v>3515.0</v>
+        <v>2.0</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6">
         <v>0.0</v>
       </c>
-      <c r="E8" s="6">
-        <v>7.0</v>
-      </c>
+      <c r="E8" s="8"/>
       <c r="F8" s="9">
-        <v>0.741479414431251</v>
+        <v>0.739904259992353</v>
       </c>
       <c r="G8" s="9">
-        <v>0.18645454168679</v>
+        <v>0.031079688357002</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>89.0</v>
+        <v>7.0</v>
       </c>
       <c r="B9" s="6">
-        <v>749.0</v>
+        <v>60.0</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" si="1"/>
@@ -702,94 +792,92 @@
       <c r="D9" s="6">
         <v>0.0</v>
       </c>
-      <c r="E9" s="6">
-        <v>2.0</v>
-      </c>
+      <c r="E9" s="8"/>
       <c r="F9" s="9">
-        <v>0.740705184405319</v>
+        <v>0.740410205109339</v>
       </c>
       <c r="G9" s="9">
-        <v>0.18645454168679</v>
+        <v>0.0237109676500874</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4">
-        <v>88.0</v>
+        <v>8.0</v>
       </c>
       <c r="B10" s="6">
-        <v>749.0</v>
+        <v>2508.0</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E10" s="6">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="F10" s="9">
-        <v>0.740280940367345</v>
+        <v>0.740159763313303</v>
       </c>
       <c r="G10" s="9">
-        <v>0.18645454168679</v>
+        <v>0.0242698346638798</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>85.0</v>
+        <v>9.0</v>
       </c>
       <c r="B11" s="6">
-        <v>746.0</v>
+        <v>3515.0</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6">
         <v>0.0</v>
       </c>
       <c r="E11" s="6">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="F11" s="9">
-        <v>0.741812651162541</v>
+        <v>0.741479414431251</v>
       </c>
       <c r="G11" s="9">
-        <v>0.186146428753938</v>
+        <v>0.18645454168679</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <v>84.0</v>
+        <v>10.0</v>
       </c>
       <c r="B12" s="6">
-        <v>726.0</v>
+        <v>12410.0</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6">
         <v>0.0</v>
       </c>
       <c r="E12" s="6">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F12" s="9">
-        <v>0.740547986202615</v>
+        <v>0.744221981703695</v>
       </c>
       <c r="G12" s="9">
-        <v>0.18514354666262</v>
+        <v>0.132923543739415</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <v>83.0</v>
+        <v>11.0</v>
       </c>
       <c r="B13" s="6">
-        <v>689.0</v>
+        <v>39.0</v>
       </c>
       <c r="C13" s="7">
         <f t="shared" si="1"/>
@@ -798,22 +886,20 @@
       <c r="D13" s="6">
         <v>0.0</v>
       </c>
-      <c r="E13" s="6">
-        <v>9.0</v>
-      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="9">
-        <v>0.740833822949908</v>
+        <v>0.740720439436135</v>
       </c>
       <c r="G13" s="9">
-        <v>0.176185322230955</v>
+        <v>0.144454965241809</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4">
-        <v>82.0</v>
+        <v>12.0</v>
       </c>
       <c r="B14" s="6">
-        <v>532.0</v>
+        <v>39.0</v>
       </c>
       <c r="C14" s="7">
         <f t="shared" si="1"/>
@@ -822,22 +908,20 @@
       <c r="D14" s="6">
         <v>0.0</v>
       </c>
-      <c r="E14" s="6">
-        <v>2.0</v>
-      </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="9">
-        <v>0.740613043251635</v>
+        <v>0.740089968187218</v>
       </c>
       <c r="G14" s="9">
-        <v>0.155404593756242</v>
+        <v>0.0229567710015223</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4">
-        <v>18.0</v>
+        <v>13.0</v>
       </c>
       <c r="B15" s="6">
-        <v>393.0</v>
+        <v>3.0</v>
       </c>
       <c r="C15" s="7">
         <f t="shared" si="1"/>
@@ -846,42 +930,44 @@
       <c r="D15" s="6">
         <v>0.0</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="9">
-        <v>0.759176024593145</v>
+        <v>0.740207651749367</v>
       </c>
       <c r="G15" s="9">
-        <v>0.149598984271116</v>
+        <v>0.0312610164773748</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4">
-        <v>1.0</v>
+        <v>14.0</v>
       </c>
       <c r="B16" s="6">
-        <v>2526.0</v>
+        <v>2.0</v>
       </c>
       <c r="C16" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="6">
         <v>0.0</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="6">
+        <v>11.0</v>
+      </c>
       <c r="F16" s="9">
-        <v>0.748215743402743</v>
+        <v>0.74011589799131</v>
       </c>
       <c r="G16" s="9">
-        <v>0.147141781022099</v>
+        <v>0.0243284287837943</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="B17" s="6">
-        <v>39.0</v>
+        <v>48.0</v>
       </c>
       <c r="C17" s="7">
         <f t="shared" si="1"/>
@@ -890,36 +976,36 @@
       <c r="D17" s="6">
         <v>0.0</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="6">
+        <v>11.0</v>
+      </c>
       <c r="F17" s="9">
-        <v>0.740720439436135</v>
+        <v>0.740848227172587</v>
       </c>
       <c r="G17" s="9">
-        <v>0.144454965241809</v>
+        <v>0.0276265952337153</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4">
-        <v>10.0</v>
+        <v>16.0</v>
       </c>
       <c r="B18" s="6">
-        <v>12410.0</v>
+        <v>91.0</v>
       </c>
       <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="6">
         <v>0.0</v>
       </c>
-      <c r="E18" s="6">
-        <v>5.0</v>
-      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="9">
-        <v>0.744221981703695</v>
+        <v>0.740241398640367</v>
       </c>
       <c r="G18" s="9">
-        <v>0.132923543739415</v>
+        <v>0.0913927878867644</v>
       </c>
     </row>
     <row r="19">
@@ -936,7 +1022,7 @@
       <c r="D19" s="6">
         <v>0.0</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="9">
         <v>0.741684000432546</v>
       </c>
@@ -946,32 +1032,32 @@
     </row>
     <row r="20">
       <c r="A20" s="4">
-        <v>28.0</v>
+        <v>18.0</v>
       </c>
       <c r="B20" s="6">
-        <v>35.0</v>
+        <v>393.0</v>
       </c>
       <c r="C20" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D20" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E20" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E20" s="10"/>
       <c r="F20" s="9">
-        <v>0.754556861717841</v>
+        <v>0.759176024593145</v>
       </c>
       <c r="G20" s="9">
-        <v>0.0924810560055265</v>
+        <v>0.149598984271116</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4">
-        <v>16.0</v>
+        <v>19.0</v>
       </c>
       <c r="B21" s="6">
-        <v>91.0</v>
+        <v>766.0</v>
       </c>
       <c r="C21" s="7">
         <f t="shared" si="1"/>
@@ -980,20 +1066,20 @@
       <c r="D21" s="6">
         <v>0.0</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="9">
-        <v>0.740241398640367</v>
+        <v>0.749728806573107</v>
       </c>
       <c r="G21" s="9">
-        <v>0.0913927878867644</v>
+        <v>0.0230581608914394</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="B22" s="6">
-        <v>295.0</v>
+        <v>862.0</v>
       </c>
       <c r="C22" s="7">
         <f t="shared" si="1"/>
@@ -1004,40 +1090,40 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
-        <v>0.740219693124285</v>
+        <v>0.742757078987824</v>
       </c>
       <c r="G22" s="9">
-        <v>0.0769716906460384</v>
+        <v>0.0227981629390395</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4">
-        <v>26.0</v>
+        <v>21.0</v>
       </c>
       <c r="B23" s="6">
-        <v>232.0</v>
+        <v>11547.0</v>
       </c>
       <c r="C23" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="6">
         <v>0.0</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="9">
-        <v>0.751879078329873</v>
+        <v>0.739853859555345</v>
       </c>
       <c r="G23" s="9">
-        <v>0.0753810186426156</v>
+        <v>0.037824954987689</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4">
-        <v>27.0</v>
+        <v>22.0</v>
       </c>
       <c r="B24" s="6">
-        <v>64.0</v>
+        <v>131.0</v>
       </c>
       <c r="C24" s="7">
         <f t="shared" si="1"/>
@@ -1046,46 +1132,42 @@
       <c r="D24" s="6">
         <v>0.0</v>
       </c>
-      <c r="E24" s="6">
-        <v>10.0</v>
-      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="9">
-        <v>0.74510552281394</v>
+        <v>0.751157277423483</v>
       </c>
       <c r="G24" s="9">
-        <v>0.0704100835786003</v>
+        <v>0.0393348458941263</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4">
-        <v>49.0</v>
+        <v>23.0</v>
       </c>
       <c r="B25" s="6">
-        <v>125584.0</v>
+        <v>37.0</v>
       </c>
       <c r="C25" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="6">
         <v>0.0</v>
       </c>
-      <c r="E25" s="6">
-        <v>6.0</v>
-      </c>
+      <c r="E25" s="10"/>
       <c r="F25" s="9">
-        <v>0.740142121457622</v>
+        <v>0.752790747399115</v>
       </c>
       <c r="G25" s="9">
-        <v>0.0557458306618616</v>
+        <v>0.0287791493366097</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4">
-        <v>25.0</v>
+        <v>24.0</v>
       </c>
       <c r="B26" s="6">
-        <v>4.0</v>
+        <v>413.0</v>
       </c>
       <c r="C26" s="7">
         <f t="shared" si="1"/>
@@ -1094,20 +1176,20 @@
       <c r="D26" s="6">
         <v>0.0</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="9">
-        <v>0.741459653321067</v>
+        <v>0.739745560362572</v>
       </c>
       <c r="G26" s="9">
-        <v>0.0441268881802902</v>
+        <v>0.0344024722967073</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4">
-        <v>48.0</v>
+        <v>25.0</v>
       </c>
       <c r="B27" s="6">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="C27" s="7">
         <f t="shared" si="1"/>
@@ -1116,44 +1198,42 @@
       <c r="D27" s="6">
         <v>0.0</v>
       </c>
-      <c r="E27" s="6">
-        <v>10.0</v>
-      </c>
+      <c r="E27" s="10"/>
       <c r="F27" s="9">
-        <v>0.739864058621702</v>
+        <v>0.741459653321067</v>
       </c>
       <c r="G27" s="9">
-        <v>0.0424714879293592</v>
+        <v>0.0441268881802902</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4">
-        <v>53.0</v>
+        <v>26.0</v>
       </c>
       <c r="B28" s="6">
-        <v>288986.0</v>
+        <v>232.0</v>
       </c>
       <c r="C28" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="6">
         <v>0.0</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="9">
-        <v>0.750405136652986</v>
+        <v>0.751879078329873</v>
       </c>
       <c r="G28" s="9">
-        <v>0.0394166603126876</v>
+        <v>0.0753810186426156</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4">
-        <v>22.0</v>
+        <v>27.0</v>
       </c>
       <c r="B29" s="6">
-        <v>131.0</v>
+        <v>64.0</v>
       </c>
       <c r="C29" s="7">
         <f t="shared" si="1"/>
@@ -1162,64 +1242,68 @@
       <c r="D29" s="6">
         <v>0.0</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="6">
+        <v>10.0</v>
+      </c>
       <c r="F29" s="9">
-        <v>0.751157277423483</v>
+        <v>0.74510552281394</v>
       </c>
       <c r="G29" s="9">
-        <v>0.0393348458941263</v>
+        <v>0.0704100835786003</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4">
-        <v>45.0</v>
+        <v>28.0</v>
       </c>
       <c r="B30" s="6">
-        <v>3.0</v>
+        <v>35.0</v>
       </c>
       <c r="C30" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D30" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E30" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="F30" s="9">
-        <v>0.746543762423178</v>
+        <v>0.754556861717841</v>
       </c>
       <c r="G30" s="9">
-        <v>0.0381540846494302</v>
+        <v>0.0924810560055265</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4">
-        <v>38.0</v>
+        <v>29.0</v>
       </c>
       <c r="B31" s="6">
-        <v>459.0</v>
+        <v>51.0</v>
       </c>
       <c r="C31" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E31" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E31" s="6">
+        <v>8.0</v>
+      </c>
       <c r="F31" s="9">
-        <v>0.740661446065883</v>
+        <v>0.744694738885608</v>
       </c>
       <c r="G31" s="9">
-        <v>0.0380425608897012</v>
+        <v>0.187370761019425</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
       <c r="B32" s="6">
-        <v>2.0</v>
+        <v>50.0</v>
       </c>
       <c r="C32" s="7">
         <f t="shared" si="1"/>
@@ -1229,18 +1313,18 @@
         <v>0.0</v>
       </c>
       <c r="E32" s="6">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="F32" s="9">
-        <v>0.741125148205752</v>
+        <v>0.741328512403892</v>
       </c>
       <c r="G32" s="9">
-        <v>0.0380418258974892</v>
+        <v>0.0227941884727096</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4">
-        <v>91.0</v>
+        <v>31.0</v>
       </c>
       <c r="B33" s="6">
         <v>3.0</v>
@@ -1252,68 +1336,66 @@
       <c r="D33" s="6">
         <v>0.0</v>
       </c>
-      <c r="E33" s="6">
-        <v>3.0</v>
-      </c>
+      <c r="E33" s="10"/>
       <c r="F33" s="9">
-        <v>0.740055157245987</v>
+        <v>0.739771561903325</v>
       </c>
       <c r="G33" s="9">
-        <v>0.0379714636465472</v>
+        <v>0.0221607323351388</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4">
-        <v>21.0</v>
+        <v>32.0</v>
       </c>
       <c r="B34" s="6">
-        <v>11547.0</v>
+        <v>2.0</v>
       </c>
       <c r="C34" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="6">
         <v>0.0</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="6">
+        <v>3.0</v>
+      </c>
       <c r="F34" s="9">
-        <v>0.739853859555345</v>
+        <v>0.745982146063207</v>
       </c>
       <c r="G34" s="9">
-        <v>0.037824954987689</v>
+        <v>0.0333550827191799</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4">
-        <v>73.0</v>
+        <v>33.0</v>
       </c>
       <c r="B35" s="6">
-        <v>23.0</v>
+        <v>250802.0</v>
       </c>
       <c r="C35" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E35" s="6">
-        <v>1.0</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="9">
-        <v>0.741525242175239</v>
+        <v>0.74131254852375</v>
       </c>
       <c r="G35" s="9">
-        <v>0.0364820917282723</v>
+        <v>0.0309853111647137</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4">
-        <v>44.0</v>
+        <v>34.0</v>
       </c>
       <c r="B36" s="6">
-        <v>717.0</v>
+        <v>100.0</v>
       </c>
       <c r="C36" s="7">
         <f t="shared" si="1"/>
@@ -1322,20 +1404,20 @@
       <c r="D36" s="6">
         <v>0.0</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="10"/>
       <c r="F36" s="9">
-        <v>0.739831141980946</v>
+        <v>0.740992871464021</v>
       </c>
       <c r="G36" s="9">
-        <v>0.0355495472908289</v>
+        <v>0.0283730484353459</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4">
-        <v>24.0</v>
+        <v>35.0</v>
       </c>
       <c r="B37" s="6">
-        <v>413.0</v>
+        <v>171.0</v>
       </c>
       <c r="C37" s="7">
         <f t="shared" si="1"/>
@@ -1344,20 +1426,20 @@
       <c r="D37" s="6">
         <v>0.0</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="9">
-        <v>0.739745560362572</v>
+        <v>0.739894511777231</v>
       </c>
       <c r="G37" s="9">
-        <v>0.0344024722967073</v>
+        <v>0.0192386204049412</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4">
-        <v>47.0</v>
+        <v>36.0</v>
       </c>
       <c r="B38" s="6">
-        <v>16648.0</v>
+        <v>17345.0</v>
       </c>
       <c r="C38" s="7">
         <f t="shared" si="1"/>
@@ -1366,20 +1448,20 @@
       <c r="D38" s="6">
         <v>0.0</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="10"/>
       <c r="F38" s="9">
-        <v>0.741638957491895</v>
+        <v>0.739747887922217</v>
       </c>
       <c r="G38" s="9">
-        <v>0.0340742356918984</v>
+        <v>0.0199731184006737</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4">
-        <v>32.0</v>
+        <v>37.0</v>
       </c>
       <c r="B39" s="6">
-        <v>2.0</v>
+        <v>42.0</v>
       </c>
       <c r="C39" s="7">
         <f t="shared" si="1"/>
@@ -1388,22 +1470,20 @@
       <c r="D39" s="6">
         <v>0.0</v>
       </c>
-      <c r="E39" s="6">
-        <v>3.0</v>
-      </c>
+      <c r="E39" s="10"/>
       <c r="F39" s="9">
-        <v>0.745982146063207</v>
+        <v>0.739825982292879</v>
       </c>
       <c r="G39" s="9">
-        <v>0.0333550827191799</v>
+        <v>0.0224520628167191</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4">
-        <v>55.0</v>
+        <v>38.0</v>
       </c>
       <c r="B40" s="6">
-        <v>988.0</v>
+        <v>459.0</v>
       </c>
       <c r="C40" s="7">
         <f t="shared" si="1"/>
@@ -1412,20 +1492,20 @@
       <c r="D40" s="6">
         <v>0.0</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="9">
-        <v>0.748795945673727</v>
+        <v>0.740661446065883</v>
       </c>
       <c r="G40" s="9">
-        <v>0.0327545775142378</v>
+        <v>0.0380425608897012</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4">
-        <v>13.0</v>
+        <v>39.0</v>
       </c>
       <c r="B41" s="6">
-        <v>3.0</v>
+        <v>128.0</v>
       </c>
       <c r="C41" s="7">
         <f t="shared" si="1"/>
@@ -1434,20 +1514,20 @@
       <c r="D41" s="6">
         <v>0.0</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="10"/>
       <c r="F41" s="9">
-        <v>0.740207651749367</v>
+        <v>0.742074146042638</v>
       </c>
       <c r="G41" s="9">
-        <v>0.0312610164773748</v>
+        <v>-0.0130381587757506</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4">
-        <v>6.0</v>
+        <v>40.0</v>
       </c>
       <c r="B42" s="6">
-        <v>2.0</v>
+        <v>41.0</v>
       </c>
       <c r="C42" s="7">
         <f t="shared" si="1"/>
@@ -1458,108 +1538,106 @@
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="9">
-        <v>0.739904259992353</v>
+        <v>0.739814967606423</v>
       </c>
       <c r="G42" s="9">
-        <v>0.031079688357002</v>
+        <v>0.0265813559639231</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4">
-        <v>51.0</v>
+        <v>41.0</v>
       </c>
       <c r="B43" s="6">
-        <v>98181.0</v>
+        <v>269.0</v>
       </c>
       <c r="C43" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="6">
         <v>0.0</v>
       </c>
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
       <c r="F43" s="9">
-        <v>0.739825579849279</v>
+        <v>0.740912271381754</v>
       </c>
       <c r="G43" s="9">
-        <v>0.0310737323937906</v>
+        <v>0.0301161064724394</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4">
-        <v>33.0</v>
+        <v>42.0</v>
       </c>
       <c r="B44" s="6">
-        <v>250802.0</v>
+        <v>18.0</v>
       </c>
       <c r="C44" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="6">
         <v>0.0</v>
       </c>
-      <c r="E44" s="8"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="9">
-        <v>0.74131254852375</v>
+        <v>0.740475932091405</v>
       </c>
       <c r="G44" s="9">
-        <v>0.0309853111647137</v>
+        <v>0.0287357123094708</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4">
-        <v>52.0</v>
+        <v>43.0</v>
       </c>
       <c r="B45" s="6">
-        <v>261178.0</v>
+        <v>268.0</v>
       </c>
       <c r="C45" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="6">
         <v>0.0</v>
       </c>
-      <c r="E45" s="8"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="9">
-        <v>0.739763749617646</v>
+        <v>0.739791166756819</v>
       </c>
       <c r="G45" s="9">
-        <v>0.0305503524482954</v>
+        <v>0.0288720920673777</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4">
-        <v>50.0</v>
+        <v>44.0</v>
       </c>
       <c r="B46" s="6">
-        <v>647413.0</v>
+        <v>717.0</v>
       </c>
       <c r="C46" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="6">
         <v>0.0</v>
       </c>
-      <c r="E46" s="6">
-        <v>6.0</v>
-      </c>
+      <c r="E46" s="10"/>
       <c r="F46" s="9">
-        <v>0.747312261909617</v>
+        <v>0.739831141980946</v>
       </c>
       <c r="G46" s="9">
-        <v>0.0305052684296592</v>
+        <v>0.0355495472908289</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4">
-        <v>58.0</v>
+        <v>45.0</v>
       </c>
       <c r="B47" s="6">
-        <v>24.0</v>
+        <v>3.0</v>
       </c>
       <c r="C47" s="7">
         <f t="shared" si="1"/>
@@ -1568,20 +1646,20 @@
       <c r="D47" s="6">
         <v>0.0</v>
       </c>
-      <c r="E47" s="8"/>
+      <c r="E47" s="10"/>
       <c r="F47" s="9">
-        <v>0.741820115814069</v>
+        <v>0.746543762423178</v>
       </c>
       <c r="G47" s="9">
-        <v>0.0302095151501275</v>
+        <v>0.0381540846494302</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4">
-        <v>41.0</v>
+        <v>46.0</v>
       </c>
       <c r="B48" s="6">
-        <v>269.0</v>
+        <v>117.0</v>
       </c>
       <c r="C48" s="7">
         <f t="shared" si="1"/>
@@ -1590,200 +1668,202 @@
       <c r="D48" s="6">
         <v>0.0</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="E48" s="10"/>
       <c r="F48" s="9">
-        <v>0.740912271381754</v>
+        <v>0.743715119047067</v>
       </c>
       <c r="G48" s="9">
-        <v>0.0301161064724394</v>
+        <v>0.0269103567242156</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4">
-        <v>62.0</v>
+        <v>47.0</v>
       </c>
       <c r="B49" s="6">
-        <v>239.0</v>
+        <v>16648.0</v>
       </c>
       <c r="C49" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="6">
         <v>0.0</v>
       </c>
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
       <c r="F49" s="9">
-        <v>0.745476523954227</v>
+        <v>0.741638957491895</v>
       </c>
       <c r="G49" s="9">
-        <v>0.0300326365210213</v>
+        <v>0.0340742356918984</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4">
-        <v>2.0</v>
+        <v>48.0</v>
       </c>
       <c r="B50" s="6">
-        <v>39404.0</v>
+        <v>14.0</v>
       </c>
       <c r="C50" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="6">
         <v>0.0</v>
       </c>
       <c r="E50" s="6">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="F50" s="9">
-        <v>0.763096570342066</v>
+        <v>0.739864058621702</v>
       </c>
       <c r="G50" s="9">
-        <v>0.0297189739520529</v>
+        <v>0.0424714879293592</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4">
-        <v>65.0</v>
+        <v>49.0</v>
       </c>
       <c r="B51" s="6">
-        <v>5.0</v>
+        <v>125584.0</v>
       </c>
       <c r="C51" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="6">
         <v>0.0</v>
       </c>
-      <c r="E51" s="8"/>
+      <c r="E51" s="6">
+        <v>6.0</v>
+      </c>
       <c r="F51" s="9">
-        <v>0.743389860135086</v>
+        <v>0.740142121457622</v>
       </c>
       <c r="G51" s="9">
-        <v>0.0291883808804943</v>
+        <v>0.0557458306618616</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4">
-        <v>43.0</v>
+        <v>50.0</v>
       </c>
       <c r="B52" s="6">
-        <v>268.0</v>
+        <v>647413.0</v>
       </c>
       <c r="C52" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="6">
         <v>0.0</v>
       </c>
-      <c r="E52" s="8"/>
+      <c r="E52" s="6">
+        <v>6.0</v>
+      </c>
       <c r="F52" s="9">
-        <v>0.739791166756819</v>
+        <v>0.747312261909617</v>
       </c>
       <c r="G52" s="9">
-        <v>0.0288720920673777</v>
+        <v>0.0305052684296592</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="4">
-        <v>23.0</v>
+        <v>51.0</v>
       </c>
       <c r="B53" s="6">
-        <v>37.0</v>
+        <v>98181.0</v>
       </c>
       <c r="C53" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="6">
         <v>0.0</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="10"/>
       <c r="F53" s="9">
-        <v>0.752790747399115</v>
+        <v>0.739825579849279</v>
       </c>
       <c r="G53" s="9">
-        <v>0.0287791493366097</v>
+        <v>0.0310737323937906</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4">
-        <v>42.0</v>
+        <v>52.0</v>
       </c>
       <c r="B54" s="6">
-        <v>18.0</v>
+        <v>261178.0</v>
       </c>
       <c r="C54" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="6">
         <v>0.0</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="E54" s="10"/>
       <c r="F54" s="9">
-        <v>0.740475932091405</v>
+        <v>0.739763749617646</v>
       </c>
       <c r="G54" s="9">
-        <v>0.0287357123094708</v>
+        <v>0.0305503524482954</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4">
-        <v>34.0</v>
+        <v>53.0</v>
       </c>
       <c r="B55" s="6">
-        <v>100.0</v>
+        <v>288986.0</v>
       </c>
       <c r="C55" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="6">
         <v>0.0</v>
       </c>
-      <c r="E55" s="8"/>
+      <c r="E55" s="10"/>
       <c r="F55" s="9">
-        <v>0.740992871464021</v>
+        <v>0.750405136652986</v>
       </c>
       <c r="G55" s="9">
-        <v>0.0283730484353459</v>
+        <v>0.0394166603126876</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4">
-        <v>15.0</v>
+        <v>54.0</v>
       </c>
       <c r="B56" s="6">
-        <v>48.0</v>
+        <v>1406.0</v>
       </c>
       <c r="C56" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" s="6">
         <v>0.0</v>
       </c>
-      <c r="E56" s="6">
-        <v>11.0</v>
-      </c>
+      <c r="E56" s="10"/>
       <c r="F56" s="9">
-        <v>0.740848227172587</v>
+        <v>0.740667829043681</v>
       </c>
       <c r="G56" s="9">
-        <v>0.0276265952337153</v>
+        <v>0.0252873696986685</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4">
-        <v>46.0</v>
+        <v>55.0</v>
       </c>
       <c r="B57" s="6">
-        <v>117.0</v>
+        <v>988.0</v>
       </c>
       <c r="C57" s="7">
         <f t="shared" si="1"/>
@@ -1792,42 +1872,42 @@
       <c r="D57" s="6">
         <v>0.0</v>
       </c>
-      <c r="E57" s="8"/>
+      <c r="E57" s="10"/>
       <c r="F57" s="9">
-        <v>0.743715119047067</v>
+        <v>0.748795945673727</v>
       </c>
       <c r="G57" s="9">
-        <v>0.0269103567242156</v>
+        <v>0.0327545775142378</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4">
-        <v>4.0</v>
+        <v>56.0</v>
       </c>
       <c r="B58" s="6">
-        <v>2.0</v>
+        <v>19.0</v>
       </c>
       <c r="C58" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D58" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="9">
-        <v>0.739754248150703</v>
+        <v>0.740298381301372</v>
       </c>
       <c r="G58" s="9">
-        <v>0.0266328097093283</v>
+        <v>0.0261071500985969</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="4">
-        <v>40.0</v>
+        <v>57.0</v>
       </c>
       <c r="B59" s="6">
-        <v>41.0</v>
+        <v>96.0</v>
       </c>
       <c r="C59" s="7">
         <f t="shared" si="1"/>
@@ -1836,64 +1916,64 @@
       <c r="D59" s="6">
         <v>0.0</v>
       </c>
-      <c r="E59" s="8"/>
+      <c r="E59" s="10"/>
       <c r="F59" s="9">
-        <v>0.739814967606423</v>
+        <v>0.739746755546436</v>
       </c>
       <c r="G59" s="9">
-        <v>0.0265813559639231</v>
+        <v>0.0211272427700812</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="4">
-        <v>59.0</v>
+        <v>58.0</v>
       </c>
       <c r="B60" s="6">
-        <v>34954.0</v>
+        <v>24.0</v>
       </c>
       <c r="C60" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="6">
         <v>0.0</v>
       </c>
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="9">
-        <v>0.739831801938552</v>
+        <v>0.741820115814069</v>
       </c>
       <c r="G60" s="9">
-        <v>0.0263665170456766</v>
+        <v>0.0302095151501275</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="4">
-        <v>56.0</v>
+        <v>59.0</v>
       </c>
       <c r="B61" s="6">
-        <v>19.0</v>
+        <v>34954.0</v>
       </c>
       <c r="C61" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E61" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E61" s="10"/>
       <c r="F61" s="9">
-        <v>0.740298381301372</v>
+        <v>0.739831801938552</v>
       </c>
       <c r="G61" s="9">
-        <v>0.0261071500985969</v>
+        <v>0.0263665170456766</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4">
-        <v>54.0</v>
+        <v>60.0</v>
       </c>
       <c r="B62" s="6">
-        <v>1406.0</v>
+        <v>259917.0</v>
       </c>
       <c r="C62" s="7">
         <f t="shared" si="1"/>
@@ -1902,42 +1982,42 @@
       <c r="D62" s="6">
         <v>0.0</v>
       </c>
-      <c r="E62" s="8"/>
+      <c r="E62" s="10"/>
       <c r="F62" s="9">
-        <v>0.740667829043681</v>
+        <v>0.740027801139258</v>
       </c>
       <c r="G62" s="9">
-        <v>0.0252873696986685</v>
+        <v>0.0183806178357539</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="4">
-        <v>71.0</v>
+        <v>61.0</v>
       </c>
       <c r="B63" s="6">
-        <v>5657.0</v>
+        <v>7.0</v>
       </c>
       <c r="C63" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E63" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E63" s="10"/>
       <c r="F63" s="9">
-        <v>0.739769001022285</v>
+        <v>0.743091663748846</v>
       </c>
       <c r="G63" s="9">
-        <v>0.0246415839789077</v>
+        <v>0.0197027217967393</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="4">
-        <v>14.0</v>
+        <v>62.0</v>
       </c>
       <c r="B64" s="6">
-        <v>2.0</v>
+        <v>239.0</v>
       </c>
       <c r="C64" s="7">
         <f t="shared" si="1"/>
@@ -1946,132 +2026,130 @@
       <c r="D64" s="6">
         <v>0.0</v>
       </c>
-      <c r="E64" s="6">
-        <v>11.0</v>
-      </c>
+      <c r="E64" s="10"/>
       <c r="F64" s="9">
-        <v>0.74011589799131</v>
+        <v>0.745476523954227</v>
       </c>
       <c r="G64" s="9">
-        <v>0.0243284287837943</v>
+        <v>0.0300326365210213</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="4">
-        <v>92.0</v>
+        <v>63.0</v>
       </c>
       <c r="B65" s="6">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C65" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D65" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E65" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E65" s="10"/>
       <c r="F65" s="9">
-        <v>0.740997070703913</v>
+        <v>0.742434783048822</v>
       </c>
       <c r="G65" s="9">
-        <v>0.0242738201225171</v>
+        <v>-0.0127911242989884</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="4">
-        <v>93.0</v>
+        <v>64.0</v>
       </c>
       <c r="B66" s="6">
-        <v>1.0</v>
+        <v>390.0</v>
       </c>
       <c r="C66" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D66" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E66" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E66" s="10"/>
       <c r="F66" s="9">
-        <v>0.740928311659923</v>
+        <v>0.741046254808785</v>
       </c>
       <c r="G66" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0217890225948516</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="4">
-        <v>94.0</v>
+        <v>65.0</v>
       </c>
       <c r="B67" s="6">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C67" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D67" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E67" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E67" s="10"/>
       <c r="F67" s="9">
-        <v>0.740800775418775</v>
+        <v>0.743389860135086</v>
       </c>
       <c r="G67" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0291883808804943</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="4">
-        <v>95.0</v>
+        <v>66.0</v>
       </c>
       <c r="B68" s="6">
-        <v>1.0</v>
+        <v>16729.0</v>
       </c>
       <c r="C68" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E68" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E68" s="10"/>
       <c r="F68" s="9">
-        <v>0.740695831329429</v>
+        <v>0.742543626181382</v>
       </c>
       <c r="G68" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0203950581440931</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="4">
-        <v>96.0</v>
+        <v>67.0</v>
       </c>
       <c r="B69" s="6">
-        <v>1.0</v>
+        <v>314.0</v>
       </c>
       <c r="C69" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D69" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E69" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E69" s="10"/>
       <c r="F69" s="9">
-        <v>0.740512765537219</v>
+        <v>0.739789638495468</v>
       </c>
       <c r="G69" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0194925210387665</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="4">
-        <v>72.0</v>
+        <v>68.0</v>
       </c>
       <c r="B70" s="6">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C70" s="7">
         <f t="shared" si="1"/>
@@ -2080,42 +2158,42 @@
       <c r="D70" s="6">
         <v>1.0</v>
       </c>
-      <c r="E70" s="8"/>
+      <c r="E70" s="10"/>
       <c r="F70" s="9">
-        <v>0.740424503631487</v>
+        <v>0.739927076828208</v>
       </c>
       <c r="G70" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0234276228348266</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="4">
-        <v>97.0</v>
+        <v>69.0</v>
       </c>
       <c r="B71" s="6">
-        <v>1.0</v>
+        <v>23.0</v>
       </c>
       <c r="C71" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D71" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E71" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E71" s="10"/>
       <c r="F71" s="9">
-        <v>0.740340838455325</v>
+        <v>0.739839449135007</v>
       </c>
       <c r="G71" s="9">
-        <v>0.0242738201225171</v>
+        <v>0.0235396155661006</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="4">
-        <v>77.0</v>
+        <v>70.0</v>
       </c>
       <c r="B72" s="6">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="C72" s="7">
         <f t="shared" si="1"/>
@@ -2124,46 +2202,42 @@
       <c r="D72" s="6">
         <v>1.0</v>
       </c>
-      <c r="E72" s="6">
-        <v>1.0</v>
-      </c>
+      <c r="E72" s="10"/>
       <c r="F72" s="9">
-        <v>0.741343955537083</v>
+        <v>0.739879195610923</v>
       </c>
       <c r="G72" s="9">
-        <v>0.0242700760024888</v>
+        <v>0.0234751644123976</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="4">
-        <v>76.0</v>
+        <v>71.0</v>
       </c>
       <c r="B73" s="6">
-        <v>23.0</v>
+        <v>5657.0</v>
       </c>
       <c r="C73" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="6">
         <v>1.0</v>
       </c>
-      <c r="E73" s="6">
-        <v>1.0</v>
-      </c>
+      <c r="E73" s="10"/>
       <c r="F73" s="9">
-        <v>0.741038326053177</v>
+        <v>0.739769001022285</v>
       </c>
       <c r="G73" s="9">
-        <v>0.0242699514311721</v>
+        <v>0.0246415839789077</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="4">
-        <v>75.0</v>
+        <v>72.0</v>
       </c>
       <c r="B74" s="6">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="C74" s="7">
         <f t="shared" si="1"/>
@@ -2172,83 +2246,81 @@
       <c r="D74" s="6">
         <v>1.0</v>
       </c>
-      <c r="E74" s="6">
-        <v>1.0</v>
-      </c>
+      <c r="E74" s="10"/>
       <c r="F74" s="9">
-        <v>0.741273784631634</v>
+        <v>0.740424503631487</v>
       </c>
       <c r="G74" s="9">
-        <v>0.0242699277916847</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="4">
-        <v>81.0</v>
+        <v>73.0</v>
       </c>
       <c r="B75" s="6">
-        <v>234.0</v>
+        <v>23.0</v>
       </c>
       <c r="C75" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D75" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E75" s="6">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="F75" s="9">
-        <v>0.74062669822008</v>
+        <v>0.741525242175239</v>
       </c>
       <c r="G75" s="9">
-        <v>0.0242699277916847</v>
+        <v>0.0364820917282723</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="4">
-        <v>80.0</v>
+        <v>74.0</v>
       </c>
       <c r="B76" s="6">
-        <v>23.0</v>
+        <v>5.0</v>
       </c>
       <c r="C76" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D76" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E76" s="6">
         <v>1.0</v>
       </c>
       <c r="F76" s="9">
-        <v>0.740037224395711</v>
+        <v>0.740010134368817</v>
       </c>
       <c r="G76" s="9">
-        <v>0.0242699277916847</v>
+        <v>0.0242578059394732</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="4">
-        <v>78.0</v>
+        <v>75.0</v>
       </c>
       <c r="B77" s="6">
-        <v>22.0</v>
+        <v>11.0</v>
       </c>
       <c r="C77" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D77" s="6">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E77" s="6">
         <v>1.0</v>
       </c>
       <c r="F77" s="9">
-        <v>0.739985679960152</v>
+        <v>0.741273784631634</v>
       </c>
       <c r="G77" s="9">
         <v>0.0242699277916847</v>
@@ -2256,7 +2328,7 @@
     </row>
     <row r="78">
       <c r="A78" s="4">
-        <v>79.0</v>
+        <v>76.0</v>
       </c>
       <c r="B78" s="6">
         <v>23.0</v>
@@ -2272,85 +2344,87 @@
         <v>1.0</v>
       </c>
       <c r="F78" s="9">
-        <v>0.74123843942218</v>
+        <v>0.741038326053177</v>
       </c>
       <c r="G78" s="9">
-        <v>0.0242698747303798</v>
+        <v>0.0242699514311721</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="4">
-        <v>8.0</v>
+        <v>77.0</v>
       </c>
       <c r="B79" s="6">
-        <v>2508.0</v>
+        <v>17.0</v>
       </c>
       <c r="C79" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="6">
         <v>1.0</v>
       </c>
       <c r="E79" s="6">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="F79" s="9">
-        <v>0.740159763313303</v>
+        <v>0.741343955537083</v>
       </c>
       <c r="G79" s="9">
-        <v>0.0242698346638798</v>
+        <v>0.0242700760024888</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="4">
-        <v>74.0</v>
+        <v>78.0</v>
       </c>
       <c r="B80" s="6">
-        <v>5.0</v>
+        <v>22.0</v>
       </c>
       <c r="C80" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D80" s="6">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E80" s="6">
         <v>1.0</v>
       </c>
       <c r="F80" s="9">
-        <v>0.740010134368817</v>
+        <v>0.739985679960152</v>
       </c>
       <c r="G80" s="9">
-        <v>0.0242578059394732</v>
+        <v>0.0242699277916847</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="4">
-        <v>7.0</v>
+        <v>79.0</v>
       </c>
       <c r="B81" s="6">
-        <v>60.0</v>
+        <v>23.0</v>
       </c>
       <c r="C81" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D81" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E81" s="10"/>
+        <v>1.0</v>
+      </c>
+      <c r="E81" s="6">
+        <v>1.0</v>
+      </c>
       <c r="F81" s="9">
-        <v>0.740410205109339</v>
+        <v>0.74123843942218</v>
       </c>
       <c r="G81" s="9">
-        <v>0.0237109676500874</v>
+        <v>0.0242698747303798</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="4">
-        <v>69.0</v>
+        <v>80.0</v>
       </c>
       <c r="B82" s="6">
         <v>23.0</v>
@@ -2362,64 +2436,70 @@
       <c r="D82" s="6">
         <v>0.0</v>
       </c>
-      <c r="E82" s="8"/>
+      <c r="E82" s="6">
+        <v>1.0</v>
+      </c>
       <c r="F82" s="9">
-        <v>0.739839449135007</v>
+        <v>0.740037224395711</v>
       </c>
       <c r="G82" s="9">
-        <v>0.0235396155661006</v>
+        <v>0.0242699277916847</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="4">
-        <v>70.0</v>
+        <v>81.0</v>
       </c>
       <c r="B83" s="6">
-        <v>1.0</v>
+        <v>234.0</v>
       </c>
       <c r="C83" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D83" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E83" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E83" s="6">
+        <v>9.0</v>
+      </c>
       <c r="F83" s="9">
-        <v>0.739879195610923</v>
+        <v>0.74062669822008</v>
       </c>
       <c r="G83" s="9">
-        <v>0.0234751644123976</v>
+        <v>0.0242699277916847</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="4">
-        <v>68.0</v>
+        <v>82.0</v>
       </c>
       <c r="B84" s="6">
-        <v>5.0</v>
+        <v>532.0</v>
       </c>
       <c r="C84" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D84" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="E84" s="8"/>
+        <v>0.0</v>
+      </c>
+      <c r="E84" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F84" s="9">
-        <v>0.739927076828208</v>
+        <v>0.740613043251635</v>
       </c>
       <c r="G84" s="9">
-        <v>0.0234276228348266</v>
+        <v>0.155404593756242</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="4">
-        <v>19.0</v>
+        <v>83.0</v>
       </c>
       <c r="B85" s="6">
-        <v>766.0</v>
+        <v>689.0</v>
       </c>
       <c r="C85" s="7">
         <f t="shared" si="1"/>
@@ -2428,20 +2508,22 @@
       <c r="D85" s="6">
         <v>0.0</v>
       </c>
-      <c r="E85" s="8"/>
+      <c r="E85" s="6">
+        <v>9.0</v>
+      </c>
       <c r="F85" s="9">
-        <v>0.749728806573107</v>
+        <v>0.740833822949908</v>
       </c>
       <c r="G85" s="9">
-        <v>0.0230581608914394</v>
+        <v>0.176185322230955</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="4">
-        <v>12.0</v>
+        <v>84.0</v>
       </c>
       <c r="B86" s="6">
-        <v>39.0</v>
+        <v>726.0</v>
       </c>
       <c r="C86" s="7">
         <f t="shared" si="1"/>
@@ -2450,20 +2532,22 @@
       <c r="D86" s="6">
         <v>0.0</v>
       </c>
-      <c r="E86" s="8"/>
+      <c r="E86" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F86" s="9">
-        <v>0.740089968187218</v>
+        <v>0.740547986202615</v>
       </c>
       <c r="G86" s="9">
-        <v>0.0229567710015223</v>
+        <v>0.18514354666262</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="4">
-        <v>20.0</v>
+        <v>85.0</v>
       </c>
       <c r="B87" s="6">
-        <v>862.0</v>
+        <v>746.0</v>
       </c>
       <c r="C87" s="7">
         <f t="shared" si="1"/>
@@ -2472,20 +2556,22 @@
       <c r="D87" s="6">
         <v>0.0</v>
       </c>
-      <c r="E87" s="8"/>
+      <c r="E87" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F87" s="9">
-        <v>0.742757078987824</v>
+        <v>0.741812651162541</v>
       </c>
       <c r="G87" s="9">
-        <v>0.0227981629390395</v>
+        <v>0.186146428753938</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="4">
-        <v>30.0</v>
+        <v>86.0</v>
       </c>
       <c r="B88" s="6">
-        <v>50.0</v>
+        <v>743.0</v>
       </c>
       <c r="C88" s="7">
         <f t="shared" si="1"/>
@@ -2495,21 +2581,21 @@
         <v>0.0</v>
       </c>
       <c r="E88" s="6">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
       <c r="F88" s="9">
-        <v>0.741328512403892</v>
+        <v>0.741128845343718</v>
       </c>
       <c r="G88" s="9">
-        <v>0.0227941884727096</v>
+        <v>0.186466811988465</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="4">
-        <v>37.0</v>
+        <v>87.0</v>
       </c>
       <c r="B89" s="6">
-        <v>42.0</v>
+        <v>749.0</v>
       </c>
       <c r="C89" s="7">
         <f t="shared" si="1"/>
@@ -2518,20 +2604,22 @@
       <c r="D89" s="6">
         <v>0.0</v>
       </c>
-      <c r="E89" s="8"/>
+      <c r="E89" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F89" s="9">
-        <v>0.739825982292879</v>
+        <v>0.741184783827072</v>
       </c>
       <c r="G89" s="9">
-        <v>0.0224520628167191</v>
+        <v>0.186470416672814</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="4">
-        <v>31.0</v>
+        <v>88.0</v>
       </c>
       <c r="B90" s="6">
-        <v>3.0</v>
+        <v>749.0</v>
       </c>
       <c r="C90" s="7">
         <f t="shared" si="1"/>
@@ -2540,20 +2628,22 @@
       <c r="D90" s="6">
         <v>0.0</v>
       </c>
-      <c r="E90" s="8"/>
+      <c r="E90" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F90" s="9">
-        <v>0.739771561903325</v>
+        <v>0.740280940367345</v>
       </c>
       <c r="G90" s="9">
-        <v>0.0221607323351388</v>
+        <v>0.18645454168679</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="4">
-        <v>64.0</v>
+        <v>89.0</v>
       </c>
       <c r="B91" s="6">
-        <v>390.0</v>
+        <v>749.0</v>
       </c>
       <c r="C91" s="7">
         <f t="shared" si="1"/>
@@ -2562,17 +2652,19 @@
       <c r="D91" s="6">
         <v>0.0</v>
       </c>
-      <c r="E91" s="8"/>
+      <c r="E91" s="6">
+        <v>2.0</v>
+      </c>
       <c r="F91" s="9">
-        <v>0.741046254808785</v>
+        <v>0.740705184405319</v>
       </c>
       <c r="G91" s="9">
-        <v>0.0217890225948516</v>
+        <v>0.18645454168679</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="4">
-        <v>5.0</v>
+        <v>90.0</v>
       </c>
       <c r="B92" s="6">
         <v>2.0</v>
@@ -2584,20 +2676,22 @@
       <c r="D92" s="6">
         <v>0.0</v>
       </c>
-      <c r="E92" s="10"/>
+      <c r="E92" s="6">
+        <v>3.0</v>
+      </c>
       <c r="F92" s="9">
-        <v>0.74211166919656</v>
+        <v>0.741125148205752</v>
       </c>
       <c r="G92" s="9">
-        <v>0.0216277064894057</v>
+        <v>0.0380418258974892</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="4">
-        <v>57.0</v>
+        <v>91.0</v>
       </c>
       <c r="B93" s="6">
-        <v>96.0</v>
+        <v>3.0</v>
       </c>
       <c r="C93" s="7">
         <f t="shared" si="1"/>
@@ -2606,152 +2700,154 @@
       <c r="D93" s="6">
         <v>0.0</v>
       </c>
-      <c r="E93" s="8"/>
+      <c r="E93" s="6">
+        <v>3.0</v>
+      </c>
       <c r="F93" s="9">
-        <v>0.739746755546436</v>
+        <v>0.740055157245987</v>
       </c>
       <c r="G93" s="9">
-        <v>0.0211272427700812</v>
+        <v>0.0379714636465472</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="4">
-        <v>66.0</v>
+        <v>92.0</v>
       </c>
       <c r="B94" s="6">
-        <v>16729.0</v>
+        <v>1.0</v>
       </c>
       <c r="C94" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E94" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E94" s="10"/>
       <c r="F94" s="9">
-        <v>0.742543626181382</v>
+        <v>0.740997070703913</v>
       </c>
       <c r="G94" s="9">
-        <v>0.0203950581440931</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="4">
-        <v>36.0</v>
+        <v>93.0</v>
       </c>
       <c r="B95" s="6">
-        <v>17345.0</v>
+        <v>1.0</v>
       </c>
       <c r="C95" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E95" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E95" s="10"/>
       <c r="F95" s="9">
-        <v>0.739747887922217</v>
+        <v>0.740928311659923</v>
       </c>
       <c r="G95" s="9">
-        <v>0.0199731184006737</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="4">
-        <v>61.0</v>
+        <v>94.0</v>
       </c>
       <c r="B96" s="6">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="C96" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D96" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E96" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E96" s="10"/>
       <c r="F96" s="9">
-        <v>0.743091663748846</v>
+        <v>0.740800775418775</v>
       </c>
       <c r="G96" s="9">
-        <v>0.0197027217967393</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="4">
-        <v>67.0</v>
+        <v>95.0</v>
       </c>
       <c r="B97" s="6">
-        <v>314.0</v>
+        <v>1.0</v>
       </c>
       <c r="C97" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D97" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E97" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E97" s="10"/>
       <c r="F97" s="9">
-        <v>0.739789638495468</v>
+        <v>0.740695831329429</v>
       </c>
       <c r="G97" s="9">
-        <v>0.0194925210387665</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="4">
-        <v>35.0</v>
+        <v>96.0</v>
       </c>
       <c r="B98" s="6">
-        <v>171.0</v>
+        <v>1.0</v>
       </c>
       <c r="C98" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D98" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E98" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E98" s="10"/>
       <c r="F98" s="9">
-        <v>0.739894511777231</v>
+        <v>0.740512765537219</v>
       </c>
       <c r="G98" s="9">
-        <v>0.0192386204049412</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="4">
-        <v>60.0</v>
+        <v>97.0</v>
       </c>
       <c r="B99" s="6">
-        <v>259917.0</v>
+        <v>1.0</v>
       </c>
       <c r="C99" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="E99" s="8"/>
+        <v>1.0</v>
+      </c>
+      <c r="E99" s="10"/>
       <c r="F99" s="9">
-        <v>0.740027801139258</v>
+        <v>0.740340838455325</v>
       </c>
       <c r="G99" s="9">
-        <v>0.0183806178357539</v>
+        <v>0.0242738201225171</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="4">
-        <v>63.0</v>
+        <v>98.0</v>
       </c>
       <c r="B100" s="6">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="C100" s="7">
         <f t="shared" si="1"/>
@@ -2760,20 +2856,22 @@
       <c r="D100" s="6">
         <v>0.0</v>
       </c>
-      <c r="E100" s="8"/>
+      <c r="E100" s="10">
+        <v>4.0</v>
+      </c>
       <c r="F100" s="9">
-        <v>0.742434783048822</v>
+        <v>0.94</v>
       </c>
       <c r="G100" s="9">
-        <v>-0.0127911242989884</v>
+        <v>0.998550282879953</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="4">
-        <v>39.0</v>
+        <v>99.0</v>
       </c>
       <c r="B101" s="6">
-        <v>128.0</v>
+        <v>2.0</v>
       </c>
       <c r="C101" s="7">
         <f t="shared" si="1"/>
@@ -2782,12 +2880,14 @@
       <c r="D101" s="6">
         <v>0.0</v>
       </c>
-      <c r="E101" s="8"/>
+      <c r="E101" s="10">
+        <v>4.0</v>
+      </c>
       <c r="F101" s="9">
-        <v>0.742074146042638</v>
+        <v>0.94</v>
       </c>
       <c r="G101" s="9">
-        <v>-0.0130381587757506</v>
+        <v>0.998550282879953</v>
       </c>
     </row>
     <row r="102">
@@ -2809,7 +2909,7 @@
     <row r="103">
       <c r="A103" s="12"/>
       <c r="C103" s="7"/>
-      <c r="E103" s="8"/>
+      <c r="E103" s="10"/>
       <c r="F103" s="13"/>
       <c r="G103" s="11"/>
     </row>
@@ -8198,9 +8298,12 @@
   </sheetData>
   <autoFilter ref="$A$1:$H$102">
     <sortState ref="A1:H102">
+      <sortCondition ref="A1:A102"/>
+      <sortCondition ref="B1:B102"/>
+      <sortCondition ref="E1:E102"/>
+      <sortCondition ref="C1:C102"/>
+      <sortCondition descending="1" ref="F1:F102"/>
       <sortCondition descending="1" ref="G1:G102"/>
-      <sortCondition descending="1" ref="F1:F102"/>
-      <sortCondition ref="A1:A102"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="C1:C102 D1:D102">
@@ -8227,9 +8330,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.63"/>
-    <col customWidth="1" min="2" max="2" width="37.5"/>
-    <col customWidth="1" min="3" max="3" width="44.0"/>
+    <col customWidth="1" min="1" max="2" width="35.63"/>
+    <col customWidth="1" min="3" max="3" width="37.5"/>
+    <col customWidth="1" min="4" max="4" width="44.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8242,86 +8345,312 @@
       <c r="C1" s="16" t="s">
         <v>10</v>
       </c>
+      <c r="D1" s="17" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="B2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="21"/>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="20"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="B5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="26"/>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="B6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="26"/>
     </row>
     <row r="7">
-      <c r="A7" s="21"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="26"/>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="26"/>
     </row>
     <row r="9">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="26"/>
     </row>
     <row r="11">
-      <c r="A11" s="21"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="26"/>
     </row>
     <row r="12">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="26"/>
     </row>
     <row r="13">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="20"/>
+      <c r="A13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="26"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="26"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+    </row>
+    <row r="29">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+    </row>
+    <row r="34">
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+    </row>
+    <row r="36">
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+    </row>
+    <row r="37">
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>